<commit_message>
Add constraints together and notTogether (initialized from excel file) and UI elements for specifying a particular year with specific number of sites. Still need to be taken into account into the routine selection.
</commit_message>
<xml_diff>
--- a/ORCHAMP_gradients_INITIALISATION.xlsx
+++ b/ORCHAMP_gradients_INITIALISATION.xlsx
@@ -243,7 +243,7 @@
     <t>VTN</t>
   </si>
   <si>
-    <t>Cervières </t>
+    <t>Cervières</t>
   </si>
   <si>
     <t>CER</t>
@@ -384,16 +384,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -509,7 +505,7 @@
   <dimension ref="1:28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -522,9 +518,10 @@
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.8744939271255"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.748987854251"/>
     <col collapsed="false" hidden="false" max="14" min="9" style="1" width="9"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -549,1130 +546,1116 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="n">
+      <c r="I1" s="2" t="n">
         <v>2020</v>
       </c>
-      <c r="J1" s="3" t="n">
+      <c r="J1" s="2" t="n">
         <v>2021</v>
       </c>
-      <c r="K1" s="3" t="n">
+      <c r="K1" s="2" t="n">
         <v>2022</v>
       </c>
-      <c r="L1" s="3" t="n">
+      <c r="L1" s="2" t="n">
         <v>2023</v>
       </c>
-      <c r="M1" s="3" t="n">
+      <c r="M1" s="2" t="n">
         <v>2024</v>
       </c>
-      <c r="N1" s="3" t="n">
+      <c r="N1" s="2" t="n">
         <v>2025</v>
       </c>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="4" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="5" t="n">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="4" t="n">
         <v>2016</v>
       </c>
-      <c r="F2" s="7" t="n">
+      <c r="F2" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="8" t="s">
+      <c r="I2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AMI2" s="0"/>
-      <c r="AMJ2" s="0"/>
-    </row>
-    <row r="3" s="4" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="L2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="5" t="n">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4" t="n">
         <v>2016</v>
       </c>
-      <c r="F3" s="7" t="n">
+      <c r="F3" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="8" t="s">
+      <c r="I3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AMI3" s="0"/>
-      <c r="AMJ3" s="0"/>
-    </row>
-    <row r="4" s="4" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="K3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="5" t="n">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="4" t="n">
         <v>2016</v>
       </c>
-      <c r="F4" s="7" t="n">
+      <c r="F4" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AMI4" s="0"/>
-      <c r="AMJ4" s="0"/>
-    </row>
-    <row r="5" s="4" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="J4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="5" t="n">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4" t="n">
         <v>2016</v>
       </c>
-      <c r="F5" s="7" t="n">
+      <c r="F5" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AMI5" s="0"/>
-      <c r="AMJ5" s="0"/>
-    </row>
-    <row r="6" s="4" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="I5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="5" t="n">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4" t="n">
         <v>2016</v>
       </c>
-      <c r="F6" s="7" t="n">
+      <c r="F6" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="8" t="s">
+      <c r="I6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AMI6" s="0"/>
-      <c r="AMJ6" s="0"/>
-    </row>
-    <row r="7" s="4" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="K6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="5" t="n">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="F7" s="7" t="n">
+      <c r="F7" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AMI7" s="0"/>
-      <c r="AMJ7" s="0"/>
-    </row>
-    <row r="8" s="4" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="I7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="5" t="n">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="F8" s="7" t="n">
+      <c r="F8" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AMI8" s="0"/>
-      <c r="AMJ8" s="0"/>
+      <c r="I8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="5" t="n">
+      <c r="D9" s="5"/>
+      <c r="E9" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="F9" s="7" t="n">
+      <c r="F9" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N9" s="6" t="s">
+      <c r="I9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="5" t="n">
+      <c r="D10" s="5"/>
+      <c r="E10" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="F10" s="7" t="n">
+      <c r="F10" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N10" s="6" t="s">
+      <c r="I10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="5" t="n">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="F11" s="7" t="n">
+      <c r="F11" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N11" s="6" t="s">
+      <c r="J11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="5" t="n">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="F12" s="7" t="n">
+      <c r="F12" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="I12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N12" s="6" t="s">
+      <c r="I12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="5" t="n">
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="F13" s="7" t="n">
+      <c r="F13" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N13" s="6" t="s">
+      <c r="I13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N13" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="5" t="n">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="F14" s="7" t="n">
+      <c r="F14" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="10" t="s">
+      <c r="I14" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="J14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K14" s="6" t="s">
+      <c r="J14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N14" s="6" t="s">
+      <c r="L14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N14" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="5" t="n">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="4" t="n">
         <v>2018</v>
       </c>
-      <c r="F15" s="5" t="n">
+      <c r="F15" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I15" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="J15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K15" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N15" s="6" t="s">
+      <c r="K15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N15" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="5" t="n">
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="4" t="n">
         <v>2018</v>
       </c>
-      <c r="F16" s="5" t="n">
+      <c r="F16" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N16" s="6" t="s">
+      <c r="I16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N16" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="5" t="n">
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="4" t="n">
         <v>2018</v>
       </c>
-      <c r="F17" s="5" t="n">
+      <c r="F17" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="I17" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N17" s="6" t="s">
+      <c r="I17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N17" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="5" t="n">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="4" t="n">
         <v>2018</v>
       </c>
-      <c r="F18" s="5" t="n">
+      <c r="F18" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="I18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N18" s="6" t="s">
+      <c r="I18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N18" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="5" t="n">
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="4" t="n">
         <v>2018</v>
       </c>
-      <c r="F19" s="5" t="n">
+      <c r="F19" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N19" s="6" t="s">
+      <c r="I19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N19" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6" t="s">
+      <c r="C20" s="5"/>
+      <c r="D20" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="5" t="n">
+      <c r="E20" s="4" t="n">
         <v>2018</v>
       </c>
-      <c r="F20" s="5" t="n">
+      <c r="F20" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="I20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N20" s="6" t="s">
+      <c r="I20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N20" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="5" t="n">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="4" t="n">
         <v>2019</v>
       </c>
-      <c r="F21" s="5" t="n">
+      <c r="F21" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="J21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N21" s="6" t="s">
+      <c r="J21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N21" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="5" t="n">
+      <c r="D22" s="5"/>
+      <c r="E22" s="4" t="n">
         <v>2019</v>
       </c>
-      <c r="F22" s="5" t="n">
+      <c r="F22" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I22" s="9" t="s">
+      <c r="I22" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="J22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N22" s="6" t="s">
+      <c r="J22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N22" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="5" t="n">
+      <c r="D23" s="5"/>
+      <c r="E23" s="4" t="n">
         <v>2019</v>
       </c>
-      <c r="F23" s="5" t="n">
+      <c r="F23" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="H23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="9" t="s">
+      <c r="I23" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="J23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N23" s="6" t="s">
+      <c r="J23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N23" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6" t="s">
+      <c r="C24" s="5"/>
+      <c r="D24" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E24" s="5" t="n">
+      <c r="E24" s="4" t="n">
         <v>2019</v>
       </c>
-      <c r="F24" s="5" t="n">
+      <c r="F24" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H24" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="I24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N24" s="6" t="s">
+      <c r="I24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N24" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="5" t="n">
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="4" t="n">
         <v>2019</v>
       </c>
-      <c r="F25" s="5" t="n">
+      <c r="F25" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H25" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I25" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L25" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M25" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N25" s="6" t="s">
+      <c r="I25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N25" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6" t="n">
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5" t="n">
         <v>2020</v>
       </c>
-      <c r="F26" s="5" t="n">
+      <c r="F26" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="G26" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="I26" s="9" t="s">
+      <c r="I26" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="J26" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M26" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N26" s="6" t="s">
+      <c r="J26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N26" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6" t="n">
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5" t="n">
         <v>2020</v>
       </c>
-      <c r="F27" s="5" t="n">
+      <c r="F27" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="I27" s="6" t="s">
+      <c r="I27" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="J27" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K27" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L27" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M27" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N27" s="6" t="s">
+      <c r="J27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N27" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6" t="n">
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5" t="n">
         <v>2020</v>
       </c>
-      <c r="F28" s="5" t="n">
+      <c r="F28" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G28" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="H28" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="I28" s="6" t="s">
+      <c r="I28" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="J28" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L28" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M28" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N28" s="6" t="s">
+      <c r="J28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N28" s="5" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Gather demi-gradient together to remove constraint.together.
</commit_message>
<xml_diff>
--- a/ORCHAMP_gradients_INITIALISATION.xlsx
+++ b/ORCHAMP_gradients_INITIALISATION.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="300" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="TABLE" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="82">
   <si>
     <t>Gradient</t>
   </si>
@@ -24,9 +24,6 @@
     <t>Code_grad</t>
   </si>
   <si>
-    <t>Paires</t>
-  </si>
-  <si>
     <t>Incomp</t>
   </si>
   <si>
@@ -117,10 +114,7 @@
     <t>VAL</t>
   </si>
   <si>
-    <t>Bauges Haut</t>
-  </si>
-  <si>
-    <t>ARM</t>
+    <t>Bauges</t>
   </si>
   <si>
     <t>ARM_PEC</t>
@@ -129,12 +123,6 @@
     <t>PNRB</t>
   </si>
   <si>
-    <t>Bauges Bas</t>
-  </si>
-  <si>
-    <t>PEC</t>
-  </si>
-  <si>
     <t>Tende</t>
   </si>
   <si>
@@ -222,19 +210,10 @@
     <t>MOU</t>
   </si>
   <si>
-    <t>Rachais</t>
-  </si>
-  <si>
-    <t>RAC</t>
+    <t>Rachais Chamechaude</t>
   </si>
   <si>
     <t>RAC_SAP</t>
-  </si>
-  <si>
-    <t>Chamechaude</t>
-  </si>
-  <si>
-    <t>SAP</t>
   </si>
   <si>
     <t>Ventoux Nord</t>
@@ -502,23 +481,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:28"/>
+  <dimension ref="1:26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.6234817813765"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.99595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="14.3765182186235"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.6275303643725"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.12550607287449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.8744939271255"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.748987854251"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="1" width="9"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.3765182186235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.6275303643725"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.12550607287449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.8744939271255"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.748987854251"/>
+    <col collapsed="false" hidden="false" max="13" min="8" style="1" width="9"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -543,392 +522,377 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
+      <c r="H1" s="2" t="n">
+        <v>2020</v>
       </c>
       <c r="I1" s="2" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="J1" s="2" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="K1" s="2" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="L1" s="2" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="M1" s="2" t="n">
-        <v>2024</v>
-      </c>
-      <c r="N1" s="2" t="n">
         <v>2025</v>
       </c>
+      <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="4" t="n">
+        <v>2016</v>
+      </c>
+      <c r="E2" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4" t="n">
-        <v>2016</v>
-      </c>
-      <c r="F2" s="6" t="n">
-        <v>6</v>
-      </c>
       <c r="G2" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>11</v>
+      <c r="I2" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>12</v>
+      <c r="K2" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="4" t="n">
+        <v>2016</v>
+      </c>
+      <c r="E3" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4" t="n">
-        <v>2016</v>
-      </c>
-      <c r="F3" s="6" t="n">
-        <v>6</v>
-      </c>
       <c r="G3" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="7" t="s">
-        <v>12</v>
+      <c r="J3" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="4" t="n">
+        <v>2016</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4" t="n">
-        <v>2016</v>
-      </c>
-      <c r="F4" s="6" t="n">
-        <v>6</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>12</v>
+      <c r="H4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="4" t="n">
+        <v>2016</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4" t="n">
-        <v>2016</v>
-      </c>
-      <c r="F5" s="6" t="n">
-        <v>6</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="4" t="n">
+        <v>2016</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4" t="n">
-        <v>2016</v>
-      </c>
-      <c r="F6" s="6" t="n">
-        <v>6</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>26</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>11</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="4" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="4" t="n">
-        <v>2017</v>
-      </c>
-      <c r="F7" s="6" t="n">
-        <v>5</v>
-      </c>
       <c r="G7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="4" t="n">
+      <c r="D8" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="F8" s="6" t="n">
+      <c r="E8" s="6" t="n">
         <v>5</v>
       </c>
+      <c r="F8" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="G8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="4" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E9" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4" t="n">
-        <v>2017</v>
-      </c>
-      <c r="F9" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>36</v>
+      <c r="H9" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="4" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="G10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4" t="n">
-        <v>2017</v>
-      </c>
-      <c r="F10" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I10" s="5" t="s">
+      <c r="H10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="5" t="s">
-        <v>11</v>
+      <c r="I10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -939,356 +903,349 @@
         <v>40</v>
       </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="4" t="n">
+      <c r="D11" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="F11" s="6" t="n">
-        <v>6</v>
+      <c r="E11" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>41</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="4" t="n">
+      <c r="D12" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="F12" s="6" t="n">
-        <v>8</v>
+      <c r="E12" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="4" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E13" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="4" t="n">
-        <v>2017</v>
-      </c>
-      <c r="F13" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="I13" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>11</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="D14" s="4" t="n">
+        <v>2018</v>
+      </c>
       <c r="E14" s="4" t="n">
-        <v>2017</v>
-      </c>
-      <c r="F14" s="6" t="n">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="J14" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="K14" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N14" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="D15" s="4" t="n">
+        <v>2018</v>
+      </c>
       <c r="E15" s="4" t="n">
-        <v>2018</v>
-      </c>
-      <c r="F15" s="4" t="n">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N15" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="4" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E16" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="4" t="n">
-        <v>2018</v>
-      </c>
-      <c r="F16" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="H16" s="5" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="D17" s="4" t="n">
+        <v>2018</v>
+      </c>
       <c r="E17" s="4" t="n">
-        <v>2018</v>
-      </c>
-      <c r="F17" s="4" t="n">
         <v>7</v>
       </c>
+      <c r="F17" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="G17" s="5" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N17" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="D18" s="4" t="n">
+        <v>2018</v>
+      </c>
       <c r="E18" s="4" t="n">
-        <v>2018</v>
-      </c>
-      <c r="F18" s="4" t="n">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N18" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="D19" s="4" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E19" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="4" t="n">
-        <v>2018</v>
-      </c>
-      <c r="F19" s="4" t="n">
-        <v>5</v>
-      </c>
       <c r="G19" s="5" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N19" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1299,244 +1256,232 @@
         <v>63</v>
       </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E20" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="4" t="n">
-        <v>2018</v>
-      </c>
-      <c r="F20" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="G20" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H20" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N20" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="D21" s="4" t="n">
+        <v>2019</v>
+      </c>
       <c r="E21" s="4" t="n">
-        <v>2019</v>
-      </c>
-      <c r="F21" s="4" t="n">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>50</v>
+        <v>18</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N21" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="D22" s="4" t="n">
+        <v>2019</v>
+      </c>
       <c r="E22" s="4" t="n">
-        <v>2019</v>
-      </c>
-      <c r="F22" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>18</v>
+        <v>6</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>50</v>
+        <v>10</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N22" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="4" t="n">
+        <v>2019</v>
+      </c>
       <c r="E23" s="4" t="n">
-        <v>2019</v>
-      </c>
-      <c r="F23" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G23" s="4" t="s">
-        <v>18</v>
+      <c r="F23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>50</v>
+        <v>10</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N23" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E24" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="4" t="n">
-        <v>2019</v>
-      </c>
-      <c r="F24" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="I24" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N24" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="5"/>
+      <c r="D25" s="5" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E25" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="4" t="n">
-        <v>2019</v>
-      </c>
-      <c r="F25" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="H25" s="5" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N25" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1547,116 +1492,35 @@
         <v>78</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5" t="n">
+      <c r="D26" s="5" t="n">
         <v>2020</v>
       </c>
-      <c r="F26" s="4" t="n">
-        <v>9</v>
+      <c r="E26" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="I26" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N26" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5" t="n">
-        <v>2020</v>
-      </c>
-      <c r="F27" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N27" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5" t="n">
-        <v>2020</v>
-      </c>
-      <c r="F28" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K28" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L28" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N28" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1688,15 +1552,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>